<commit_message>
Made the Property layer non-default in the Process View
</commit_message>
<xml_diff>
--- a/doc/Nodes and Edges.xlsx
+++ b/doc/Nodes and Edges.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Core FTG+PM" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -204,8 +207,36 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -483,7 +514,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>